<commit_message>
Code updates has beed done
</commit_message>
<xml_diff>
--- a/TestData/ApplicationPro_DataFeed.xlsx
+++ b/TestData/ApplicationPro_DataFeed.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srinivasa.punnam\OneDrive - Sapiens\Desktop\Prasad Punnam\Testing\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srinivasa.punnam\PycharmProjects\ApplicationPro\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC6EA890-676F-4FA6-A9D4-11352E3231EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84E475D3-B89A-4CBF-95B9-CE9C891A2C6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{D409B3C3-83F5-4FB1-9D92-4899A37DC1FC}"/>
   </bookViews>
@@ -17,6 +17,7 @@
     <sheet name="LoginPage" sheetId="1" r:id="rId2"/>
     <sheet name="CreateNewApplication" sheetId="2" r:id="rId3"/>
     <sheet name="PrimaryInsured" sheetId="4" r:id="rId4"/>
+    <sheet name="ProductSelection" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="383">
   <si>
     <t>UserName</t>
   </si>
@@ -213,6 +214,981 @@
   </si>
   <si>
     <t>Married</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Citizenship</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Alabama</t>
+  </si>
+  <si>
+    <t>Alaska</t>
+  </si>
+  <si>
+    <t>Arizona</t>
+  </si>
+  <si>
+    <t>Arkansas</t>
+  </si>
+  <si>
+    <t>California</t>
+  </si>
+  <si>
+    <t>Colorado</t>
+  </si>
+  <si>
+    <t>Connecticut</t>
+  </si>
+  <si>
+    <t>Delaware</t>
+  </si>
+  <si>
+    <t>District of Columbia</t>
+  </si>
+  <si>
+    <t>Georgia</t>
+  </si>
+  <si>
+    <t>Guam</t>
+  </si>
+  <si>
+    <t>Hawaii</t>
+  </si>
+  <si>
+    <t>Idaho</t>
+  </si>
+  <si>
+    <t>Indiana</t>
+  </si>
+  <si>
+    <t>Iowa</t>
+  </si>
+  <si>
+    <t>Kansas</t>
+  </si>
+  <si>
+    <t>Kentucky</t>
+  </si>
+  <si>
+    <t>Louisiana</t>
+  </si>
+  <si>
+    <t>Maine</t>
+  </si>
+  <si>
+    <t>Maryland</t>
+  </si>
+  <si>
+    <t>Massachusetts</t>
+  </si>
+  <si>
+    <t>Michigan</t>
+  </si>
+  <si>
+    <t>Minnesota</t>
+  </si>
+  <si>
+    <t>Mississippi</t>
+  </si>
+  <si>
+    <t>Missouri</t>
+  </si>
+  <si>
+    <t>Montana</t>
+  </si>
+  <si>
+    <t>Nebraska</t>
+  </si>
+  <si>
+    <t>Nevada</t>
+  </si>
+  <si>
+    <t>New Hampshire</t>
+  </si>
+  <si>
+    <t>New Jersey</t>
+  </si>
+  <si>
+    <t>New Mexico</t>
+  </si>
+  <si>
+    <t>New York</t>
+  </si>
+  <si>
+    <t>North Carolina</t>
+  </si>
+  <si>
+    <t>North Dakota</t>
+  </si>
+  <si>
+    <t>Ohio</t>
+  </si>
+  <si>
+    <t>Oklahoma</t>
+  </si>
+  <si>
+    <t>Oregon</t>
+  </si>
+  <si>
+    <t>Pennsylvania</t>
+  </si>
+  <si>
+    <t>Puerto Rico</t>
+  </si>
+  <si>
+    <t>Rhode Island</t>
+  </si>
+  <si>
+    <t>South Carolina</t>
+  </si>
+  <si>
+    <t>South Dakota</t>
+  </si>
+  <si>
+    <t>Tennessee</t>
+  </si>
+  <si>
+    <t>Texas</t>
+  </si>
+  <si>
+    <t>Utah</t>
+  </si>
+  <si>
+    <t>Vermont</t>
+  </si>
+  <si>
+    <t>Virgin Islands</t>
+  </si>
+  <si>
+    <t>Virginia</t>
+  </si>
+  <si>
+    <t>Washington</t>
+  </si>
+  <si>
+    <t>West Virginia</t>
+  </si>
+  <si>
+    <t>Wisconsin</t>
+  </si>
+  <si>
+    <t>Wyoming</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>U.S. Citizen</t>
+  </si>
+  <si>
+    <t>United States Of America</t>
+  </si>
+  <si>
+    <t>Afghanistan</t>
+  </si>
+  <si>
+    <t>Aland Islands</t>
+  </si>
+  <si>
+    <t>Albania</t>
+  </si>
+  <si>
+    <t>Algeria</t>
+  </si>
+  <si>
+    <t>American Samoa</t>
+  </si>
+  <si>
+    <t>Andorra</t>
+  </si>
+  <si>
+    <t>Angola</t>
+  </si>
+  <si>
+    <t>Anguilla</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Antarctica </t>
+  </si>
+  <si>
+    <t>Antigua and Barbuda</t>
+  </si>
+  <si>
+    <t>Argentina</t>
+  </si>
+  <si>
+    <t>Armenia</t>
+  </si>
+  <si>
+    <t>Aruba</t>
+  </si>
+  <si>
+    <t>Ascension Islands</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>Austria</t>
+  </si>
+  <si>
+    <t>Azerbaijan</t>
+  </si>
+  <si>
+    <t>Bahamas</t>
+  </si>
+  <si>
+    <t>Bahrain</t>
+  </si>
+  <si>
+    <t>Bangladesh</t>
+  </si>
+  <si>
+    <t>Barbados</t>
+  </si>
+  <si>
+    <t>Belarus</t>
+  </si>
+  <si>
+    <t>Belgium</t>
+  </si>
+  <si>
+    <t>Belize</t>
+  </si>
+  <si>
+    <t>Benin</t>
+  </si>
+  <si>
+    <t>Bermuda</t>
+  </si>
+  <si>
+    <t>Bhutan</t>
+  </si>
+  <si>
+    <t>Bolivia</t>
+  </si>
+  <si>
+    <t>Bonaire, Sint Eustatius and Saba</t>
+  </si>
+  <si>
+    <t>Bosnia and Herzegovina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Botswana </t>
+  </si>
+  <si>
+    <t>Bouvet Island</t>
+  </si>
+  <si>
+    <t>Brazil</t>
+  </si>
+  <si>
+    <t>British Indian Ocean Territory</t>
+  </si>
+  <si>
+    <t>Brunei</t>
+  </si>
+  <si>
+    <t>Bulgaria</t>
+  </si>
+  <si>
+    <t>Burkina Faso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Burma (Union Of Myanmar) </t>
+  </si>
+  <si>
+    <t>Burundi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cambodia </t>
+  </si>
+  <si>
+    <t>Cameroon</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>Cape Verde</t>
+  </si>
+  <si>
+    <t>Cayman Islands</t>
+  </si>
+  <si>
+    <t>Central African Republic</t>
+  </si>
+  <si>
+    <t>Chad</t>
+  </si>
+  <si>
+    <t>Chile</t>
+  </si>
+  <si>
+    <t>China</t>
+  </si>
+  <si>
+    <t>Christmas Island</t>
+  </si>
+  <si>
+    <t>Cocoa Islands</t>
+  </si>
+  <si>
+    <t>Cocos (Keeling) Islands</t>
+  </si>
+  <si>
+    <t>Colombia</t>
+  </si>
+  <si>
+    <t>Comoros</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Congo </t>
+  </si>
+  <si>
+    <t>Cook Islands</t>
+  </si>
+  <si>
+    <t>Costa Rica</t>
+  </si>
+  <si>
+    <t>Cote d'Ivoire</t>
+  </si>
+  <si>
+    <t>Croatia</t>
+  </si>
+  <si>
+    <t>Cuba</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Curacao </t>
+  </si>
+  <si>
+    <t>Cyprus</t>
+  </si>
+  <si>
+    <t>Czech Republic</t>
+  </si>
+  <si>
+    <t>Czechoslovakia</t>
+  </si>
+  <si>
+    <t>Democratic Republic of the Congo</t>
+  </si>
+  <si>
+    <t>Denmark</t>
+  </si>
+  <si>
+    <t>Diego Garcia</t>
+  </si>
+  <si>
+    <t>Djibouti</t>
+  </si>
+  <si>
+    <t>Dominica</t>
+  </si>
+  <si>
+    <t>Dominican Republic</t>
+  </si>
+  <si>
+    <t>Ecuador</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Egypt </t>
+  </si>
+  <si>
+    <t>El Salvador</t>
+  </si>
+  <si>
+    <t>Equatorial Guine</t>
+  </si>
+  <si>
+    <t>Eritrea</t>
+  </si>
+  <si>
+    <t>Estonia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ethiopia </t>
+  </si>
+  <si>
+    <t>Falkland Islands</t>
+  </si>
+  <si>
+    <t>Faroe Islands</t>
+  </si>
+  <si>
+    <t>Federated States of Micronesia</t>
+  </si>
+  <si>
+    <t>Fiji</t>
+  </si>
+  <si>
+    <t>Finland</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>French Guiana</t>
+  </si>
+  <si>
+    <t>French Polynesi</t>
+  </si>
+  <si>
+    <t>French Southern Territories</t>
+  </si>
+  <si>
+    <t>Gabon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gambia </t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>Ghana</t>
+  </si>
+  <si>
+    <t>Gibraltar</t>
+  </si>
+  <si>
+    <t>Greece</t>
+  </si>
+  <si>
+    <t>Greenland</t>
+  </si>
+  <si>
+    <t>Grenada</t>
+  </si>
+  <si>
+    <t>Guadeloupe</t>
+  </si>
+  <si>
+    <t>Guatemala</t>
+  </si>
+  <si>
+    <t>Guernsey</t>
+  </si>
+  <si>
+    <t>Guinea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Guinea-Bissau </t>
+  </si>
+  <si>
+    <t>Guyana</t>
+  </si>
+  <si>
+    <t>Haiti</t>
+  </si>
+  <si>
+    <t>Haiti-Gourde</t>
+  </si>
+  <si>
+    <t>Heard Island and McDonald Islands</t>
+  </si>
+  <si>
+    <t>Holy See (Vatican City State)</t>
+  </si>
+  <si>
+    <t>Honduras</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hong Kong </t>
+  </si>
+  <si>
+    <t>Hungary</t>
+  </si>
+  <si>
+    <t>Iceland</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Indonesia</t>
+  </si>
+  <si>
+    <t>Iraq</t>
+  </si>
+  <si>
+    <t>Ireland</t>
+  </si>
+  <si>
+    <t>Islamic Republic of Iran</t>
+  </si>
+  <si>
+    <t>Isle of Man</t>
+  </si>
+  <si>
+    <t>Israel</t>
+  </si>
+  <si>
+    <t>Italy</t>
+  </si>
+  <si>
+    <t>Ivory Coast, Republic Of</t>
+  </si>
+  <si>
+    <t>Jamaica</t>
+  </si>
+  <si>
+    <t>Japan</t>
+  </si>
+  <si>
+    <t>Jersey</t>
+  </si>
+  <si>
+    <t>Jordan</t>
+  </si>
+  <si>
+    <t>Kazakhstan</t>
+  </si>
+  <si>
+    <t>Kenya</t>
+  </si>
+  <si>
+    <t>Kiribati</t>
+  </si>
+  <si>
+    <t>Korea</t>
+  </si>
+  <si>
+    <t>Kosovo</t>
+  </si>
+  <si>
+    <t>Kuwait</t>
+  </si>
+  <si>
+    <t>Kyrgyzstan</t>
+  </si>
+  <si>
+    <t>Lao People's Democratic Republic</t>
+  </si>
+  <si>
+    <t>Latvia</t>
+  </si>
+  <si>
+    <t>Lebanon</t>
+  </si>
+  <si>
+    <t>Lesotho</t>
+  </si>
+  <si>
+    <t>Liberia</t>
+  </si>
+  <si>
+    <t>Libya</t>
+  </si>
+  <si>
+    <t>Liechtenstein</t>
+  </si>
+  <si>
+    <t>Lithuania</t>
+  </si>
+  <si>
+    <t>Luxembourg</t>
+  </si>
+  <si>
+    <t>Macao</t>
+  </si>
+  <si>
+    <t>Macedonia</t>
+  </si>
+  <si>
+    <t>Madagascar</t>
+  </si>
+  <si>
+    <t>Malawi</t>
+  </si>
+  <si>
+    <t>Malaysia</t>
+  </si>
+  <si>
+    <t>Maldives</t>
+  </si>
+  <si>
+    <t>Mali</t>
+  </si>
+  <si>
+    <t>Malta</t>
+  </si>
+  <si>
+    <t>Marshall Islands</t>
+  </si>
+  <si>
+    <t>Martinique</t>
+  </si>
+  <si>
+    <t>Mauritania</t>
+  </si>
+  <si>
+    <t>Mauritius</t>
+  </si>
+  <si>
+    <t>Mayotte</t>
+  </si>
+  <si>
+    <t>Mexico</t>
+  </si>
+  <si>
+    <t>Moldova</t>
+  </si>
+  <si>
+    <t>Monaco</t>
+  </si>
+  <si>
+    <t>Mongolia</t>
+  </si>
+  <si>
+    <t>Montenegro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Montserrat </t>
+  </si>
+  <si>
+    <t>Morocco</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mozambique </t>
+  </si>
+  <si>
+    <t>Myanmar</t>
+  </si>
+  <si>
+    <t>Namibia</t>
+  </si>
+  <si>
+    <t>Nauru</t>
+  </si>
+  <si>
+    <t>Nepal</t>
+  </si>
+  <si>
+    <t>Netherland Antilles</t>
+  </si>
+  <si>
+    <t>Netherlands</t>
+  </si>
+  <si>
+    <t>New Caledonia</t>
+  </si>
+  <si>
+    <t>New Zealand</t>
+  </si>
+  <si>
+    <t>Nicaragua</t>
+  </si>
+  <si>
+    <t>Niger</t>
+  </si>
+  <si>
+    <t>Nigeria</t>
+  </si>
+  <si>
+    <t>Norfolk Island</t>
+  </si>
+  <si>
+    <t>North Korea</t>
+  </si>
+  <si>
+    <t>North Yemen</t>
+  </si>
+  <si>
+    <t>Northern Mariana Islands</t>
+  </si>
+  <si>
+    <t>Norway</t>
+  </si>
+  <si>
+    <t>Oman</t>
+  </si>
+  <si>
+    <t>Pakistan</t>
+  </si>
+  <si>
+    <t>Panama</t>
+  </si>
+  <si>
+    <t>Papua New Guinea</t>
+  </si>
+  <si>
+    <t>Paraguay</t>
+  </si>
+  <si>
+    <t>PERU</t>
+  </si>
+  <si>
+    <t>Philippines</t>
+  </si>
+  <si>
+    <t>Pitcairn</t>
+  </si>
+  <si>
+    <t>Poland</t>
+  </si>
+  <si>
+    <t>Portugal</t>
+  </si>
+  <si>
+    <t>Qatar</t>
+  </si>
+  <si>
+    <t>Reunion</t>
+  </si>
+  <si>
+    <t>Romania</t>
+  </si>
+  <si>
+    <t>Russia</t>
+  </si>
+  <si>
+    <t>Rwanda</t>
+  </si>
+  <si>
+    <t>Saint Helena, Ascension and Tristan da Cunha</t>
+  </si>
+  <si>
+    <t>Saint Kitts and Nevis</t>
+  </si>
+  <si>
+    <t>Saint Lucia</t>
+  </si>
+  <si>
+    <t>Saint Martin (French Part)</t>
+  </si>
+  <si>
+    <t>Saint Pierre and Miquelon</t>
+  </si>
+  <si>
+    <t>Saint Vincent and the Grenadines</t>
+  </si>
+  <si>
+    <t>San Marino</t>
+  </si>
+  <si>
+    <t>Sao Tome and Principe</t>
+  </si>
+  <si>
+    <t>Serbia</t>
+  </si>
+  <si>
+    <t>Seychelles</t>
+  </si>
+  <si>
+    <t>Sierra Leone</t>
+  </si>
+  <si>
+    <t>Singapore</t>
+  </si>
+  <si>
+    <t>Slovakia</t>
+  </si>
+  <si>
+    <t>Slovenia</t>
+  </si>
+  <si>
+    <t>Solomon Islands</t>
+  </si>
+  <si>
+    <t>Somalia</t>
+  </si>
+  <si>
+    <t>South Africa</t>
+  </si>
+  <si>
+    <t>South Georgia and the South Sandwich Island</t>
+  </si>
+  <si>
+    <t>South Korea</t>
+  </si>
+  <si>
+    <t>South Sudan</t>
+  </si>
+  <si>
+    <t>South Yemen</t>
+  </si>
+  <si>
+    <t>Spain</t>
+  </si>
+  <si>
+    <t>Sri Lanka</t>
+  </si>
+  <si>
+    <t>Suriname</t>
+  </si>
+  <si>
+    <t>Swaziland</t>
+  </si>
+  <si>
+    <t>Sweden</t>
+  </si>
+  <si>
+    <t>Switzerland</t>
+  </si>
+  <si>
+    <t>Syrian Arab Republic</t>
+  </si>
+  <si>
+    <t>Taiwan</t>
+  </si>
+  <si>
+    <t>Tajikistan</t>
+  </si>
+  <si>
+    <t>Tanzania, United Republic of</t>
+  </si>
+  <si>
+    <t>Thailand</t>
+  </si>
+  <si>
+    <t>Timor-Leste</t>
+  </si>
+  <si>
+    <t>Togo</t>
+  </si>
+  <si>
+    <t>Tokelau</t>
+  </si>
+  <si>
+    <t>Tonga</t>
+  </si>
+  <si>
+    <t>Tunisia</t>
+  </si>
+  <si>
+    <t>Turkey</t>
+  </si>
+  <si>
+    <t>Turks and Caicos Islands</t>
+  </si>
+  <si>
+    <t>Uganda</t>
+  </si>
+  <si>
+    <t>Ukraine</t>
+  </si>
+  <si>
+    <t>Union of Soviet Socialist Republics</t>
+  </si>
+  <si>
+    <t>United Arab Emirates</t>
+  </si>
+  <si>
+    <t>United Kingdom</t>
+  </si>
+  <si>
+    <t>United States Minor Outlying Islands</t>
+  </si>
+  <si>
+    <t>Uruguay</t>
+  </si>
+  <si>
+    <t>Uzbekistan</t>
+  </si>
+  <si>
+    <t>Vanuatu</t>
+  </si>
+  <si>
+    <t>Venezuela</t>
+  </si>
+  <si>
+    <t>Vietnam</t>
+  </si>
+  <si>
+    <t>Virgin Islands, British</t>
+  </si>
+  <si>
+    <t>Virgin Islands, US</t>
+  </si>
+  <si>
+    <t>Wallis and Futun</t>
+  </si>
+  <si>
+    <t>Western Sahara</t>
+  </si>
+  <si>
+    <t>Western Samoa</t>
+  </si>
+  <si>
+    <t>Yemen</t>
+  </si>
+  <si>
+    <t>Yugoslavia</t>
+  </si>
+  <si>
+    <t>Zaire</t>
+  </si>
+  <si>
+    <t>Zambia</t>
+  </si>
+  <si>
+    <t>Zimbabwe</t>
+  </si>
+  <si>
+    <t>Tobacco</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Work_Status</t>
+  </si>
+  <si>
+    <t>Occupational_Duties</t>
+  </si>
+  <si>
+    <t>Employer_Name</t>
+  </si>
+  <si>
+    <t>Employer_Address_Line_1</t>
+  </si>
+  <si>
+    <t>Employer_Address_Line_2</t>
+  </si>
+  <si>
+    <t>Country_of_Birth</t>
+  </si>
+  <si>
+    <t>State_of_Birth</t>
+  </si>
+  <si>
+    <t>Driver_License_Number</t>
+  </si>
+  <si>
+    <t>State_of_Issue</t>
+  </si>
+  <si>
+    <t>DIRIUT 28376423874</t>
+  </si>
+  <si>
+    <t>Employed</t>
+  </si>
+  <si>
+    <t>ACCOUNTANT</t>
+  </si>
+  <si>
+    <t>Deutsche Bank</t>
+  </si>
+  <si>
+    <t>Deutsche Line 1</t>
+  </si>
+  <si>
+    <t>Deutsche Line 2</t>
+  </si>
+  <si>
+    <t>Deutsche City</t>
+  </si>
+  <si>
+    <t>End</t>
   </si>
 </sst>
 </file>
@@ -257,9 +1233,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -595,85 +1572,1503 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D93354D-29BE-434F-A938-52974A195CF5}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:D254"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C254"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="31" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
       <c r="B1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>18</v>
       </c>
       <c r="B2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>19</v>
       </c>
       <c r="B3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>20</v>
       </c>
       <c r="B4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>21</v>
       </c>
       <c r="B5" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
+        <v>118</v>
+      </c>
+      <c r="D5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
       <c r="B6" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>119</v>
+      </c>
+      <c r="D6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>22</v>
       </c>
       <c r="B7" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C7" t="s">
+        <v>120</v>
+      </c>
+      <c r="D7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>23</v>
       </c>
       <c r="B8" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>121</v>
+      </c>
+      <c r="D8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>31</v>
+      </c>
+      <c r="C9" t="s">
+        <v>122</v>
+      </c>
+      <c r="D9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>123</v>
+      </c>
+      <c r="D10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C11" t="s">
+        <v>124</v>
+      </c>
+      <c r="D11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C12" t="s">
+        <v>125</v>
+      </c>
+      <c r="D12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C13" t="s">
+        <v>126</v>
+      </c>
+      <c r="D13" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C14" t="s">
+        <v>127</v>
+      </c>
+      <c r="D14" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C15" t="s">
+        <v>128</v>
+      </c>
+      <c r="D15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C16" t="s">
+        <v>129</v>
+      </c>
+      <c r="D16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C17" t="s">
+        <v>130</v>
+      </c>
+      <c r="D17" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C18" t="s">
+        <v>131</v>
+      </c>
+      <c r="D18" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C19" t="s">
+        <v>132</v>
+      </c>
+      <c r="D19" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C20" t="s">
+        <v>133</v>
+      </c>
+      <c r="D20" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="21" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C21" t="s">
+        <v>134</v>
+      </c>
+      <c r="D21" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="22" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C22" t="s">
+        <v>135</v>
+      </c>
+      <c r="D22" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="23" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C23" t="s">
+        <v>136</v>
+      </c>
+      <c r="D23" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="24" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C24" t="s">
+        <v>137</v>
+      </c>
+      <c r="D24" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="25" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C25" t="s">
+        <v>138</v>
+      </c>
+      <c r="D25" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="26" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C26" t="s">
+        <v>139</v>
+      </c>
+      <c r="D26" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="27" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C27" t="s">
+        <v>140</v>
+      </c>
+      <c r="D27" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="28" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C28" t="s">
+        <v>141</v>
+      </c>
+      <c r="D28" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="29" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C29" t="s">
+        <v>142</v>
+      </c>
+      <c r="D29" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="30" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C30" t="s">
+        <v>143</v>
+      </c>
+      <c r="D30" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="31" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C31" t="s">
+        <v>144</v>
+      </c>
+      <c r="D31" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="32" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C32" t="s">
+        <v>145</v>
+      </c>
+      <c r="D32" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="33" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C33" t="s">
+        <v>146</v>
+      </c>
+      <c r="D33" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="34" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C34" t="s">
+        <v>147</v>
+      </c>
+      <c r="D34" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="35" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C35" t="s">
+        <v>148</v>
+      </c>
+      <c r="D35" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="36" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C36" t="s">
+        <v>149</v>
+      </c>
+      <c r="D36" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="37" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C37" t="s">
+        <v>150</v>
+      </c>
+      <c r="D37" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="38" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C38" t="s">
+        <v>151</v>
+      </c>
+      <c r="D38" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="39" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C39" t="s">
+        <v>152</v>
+      </c>
+      <c r="D39" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="40" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C40" t="s">
+        <v>153</v>
+      </c>
+      <c r="D40" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="41" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C41" t="s">
+        <v>154</v>
+      </c>
+      <c r="D41" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="42" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C42" t="s">
+        <v>155</v>
+      </c>
+      <c r="D42" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="43" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C43" t="s">
+        <v>156</v>
+      </c>
+      <c r="D43" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="44" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C44" t="s">
+        <v>157</v>
+      </c>
+      <c r="D44" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="45" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C45" t="s">
+        <v>158</v>
+      </c>
+      <c r="D45" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="46" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C46" t="s">
+        <v>159</v>
+      </c>
+      <c r="D46" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="47" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C47" t="s">
+        <v>160</v>
+      </c>
+      <c r="D47" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="48" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C48" t="s">
+        <v>161</v>
+      </c>
+      <c r="D48" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="49" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C49" t="s">
+        <v>162</v>
+      </c>
+      <c r="D49" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="50" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C50" t="s">
+        <v>163</v>
+      </c>
+      <c r="D50" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="51" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C51" t="s">
+        <v>164</v>
+      </c>
+      <c r="D51" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="52" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C52" t="s">
+        <v>165</v>
+      </c>
+      <c r="D52" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="53" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C53" t="s">
+        <v>166</v>
+      </c>
+      <c r="D53" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="54" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C54" t="s">
+        <v>167</v>
+      </c>
+      <c r="D54" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="55" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C55" t="s">
+        <v>168</v>
+      </c>
+      <c r="D55" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="56" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C56" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="57" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C57" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="58" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C58" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="59" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C59" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="60" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C60" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="61" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C61" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="62" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C62" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="63" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C63" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="64" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C64" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="65" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C65" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="66" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C66" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="67" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C67" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="68" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C68" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="69" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C69" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="70" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C70" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="71" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C71" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="72" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C72" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="73" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C73" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="74" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C74" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="75" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C75" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="76" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C76" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="77" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C77" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="78" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C78" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="79" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C79" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="80" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C80" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="81" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C81" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="82" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C82" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="83" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C83" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="84" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C84" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="85" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C85" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="86" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C86" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="87" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C87" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="88" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C88" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="89" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C89" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="90" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C90" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="91" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C91" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="92" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C92" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="93" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C93" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="94" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C94" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="95" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C95" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="96" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C96" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="97" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C97" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="98" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C98" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="99" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C99" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="100" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C100" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="101" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C101" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="102" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C102" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="103" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C103" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="104" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C104" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="105" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C105" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="106" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C106" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="107" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C107" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="108" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C108" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="109" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C109" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="110" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C110" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="111" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C111" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="112" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C112" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="113" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C113" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="114" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C114" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="115" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C115" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="116" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C116" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="117" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C117" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="118" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C118" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="119" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C119" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="120" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C120" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="121" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C121" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="122" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C122" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="123" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C123" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="124" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C124" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="125" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C125" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="126" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C126" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="127" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C127" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="128" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C128" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="129" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C129" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="130" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C130" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="131" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C131" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="132" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C132" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="133" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C133" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="134" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C134" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="135" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C135" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="136" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C136" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="137" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C137" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="138" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C138" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="139" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C139" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="140" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C140" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="141" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C141" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="142" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C142" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="143" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C143" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="144" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C144" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="145" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C145" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="146" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C146" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="147" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C147" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="148" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C148" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="149" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C149" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="150" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C150" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="151" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C151" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="152" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C152" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="153" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C153" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="154" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C154" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="155" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C155" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="156" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C156" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="157" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C157" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="158" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C158" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="159" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C159" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="160" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C160" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="161" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C161" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="162" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C162" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="163" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C163" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="164" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C164" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="165" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C165" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="166" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C166" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="167" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C167" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="168" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C168" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="169" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C169" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="170" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C170" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="171" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C171" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="172" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C172" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="173" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C173" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="174" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C174" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="175" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C175" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="176" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C176" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="177" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C177" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="178" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C178" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="179" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C179" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="180" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C180" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="181" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C181" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="182" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C182" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="183" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C183" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="184" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C184" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="185" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C185" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="186" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C186" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="187" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C187" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="188" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C188" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="189" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C189" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="190" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C190" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="191" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C191" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="192" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C192" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="193" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C193" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="194" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C194" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="195" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C195" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="196" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C196" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="197" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C197" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="198" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C198" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="199" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C199" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="200" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C200" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="201" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C201" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="202" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C202" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="203" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C203" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="204" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C204" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="205" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C205" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="206" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C206" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="207" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C207" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="208" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C208" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="209" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C209" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="210" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C210" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="211" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C211" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="212" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C212" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="213" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C213" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="214" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C214" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="215" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C215" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="216" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C216" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="217" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C217" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="218" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C218" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="219" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C219" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="220" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C220" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="221" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C221" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="222" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C222" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="223" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C223" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="224" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C224" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="225" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C225" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="226" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C226" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="227" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C227" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="228" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C228" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="229" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C229" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="230" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C230" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="231" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C231" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="232" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C232" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="233" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C233" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="234" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C234" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="235" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C235" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="236" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C236" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="237" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C237" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="238" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C238" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="239" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C239" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="240" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C240" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="241" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C241" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="242" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C242" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="243" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C243" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="244" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C244" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="245" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C245" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="246" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C246" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="247" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C247" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="248" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C248" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="249" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C249" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="250" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C250" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="251" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C251" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="252" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C252" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="253" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C253" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="254" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C254" t="s">
+        <v>363</v>
       </c>
     </row>
   </sheetData>
@@ -852,17 +3247,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{573F1447-AAF6-44E3-84EB-841D47BD4BB3}">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:AF3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="T3" sqref="T3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.77734375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.33203125" bestFit="1" customWidth="1"/>
@@ -870,14 +3265,28 @@
     <col min="9" max="9" width="11.109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="25.21875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.21875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="6.21875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="22" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="12" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="14.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>38</v>
       </c>
@@ -926,8 +3335,56 @@
       <c r="P1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q1" t="s">
+        <v>364</v>
+      </c>
+      <c r="R1" t="s">
+        <v>366</v>
+      </c>
+      <c r="S1" t="s">
+        <v>58</v>
+      </c>
+      <c r="T1" t="s">
+        <v>367</v>
+      </c>
+      <c r="U1" t="s">
+        <v>368</v>
+      </c>
+      <c r="V1" t="s">
+        <v>369</v>
+      </c>
+      <c r="W1" t="s">
+        <v>370</v>
+      </c>
+      <c r="X1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>371</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>372</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>373</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>374</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -938,14 +3395,20 @@
         <v>40</v>
       </c>
       <c r="D2" t="s">
-        <v>54</v>
+        <v>104</v>
       </c>
       <c r="E2">
-        <v>67676</v>
+        <v>34534</v>
       </c>
       <c r="F2">
         <v>6756756765</v>
       </c>
+      <c r="G2" t="s">
+        <v>113</v>
+      </c>
+      <c r="H2" t="s">
+        <v>113</v>
+      </c>
       <c r="I2">
         <v>6756756765</v>
       </c>
@@ -964,11 +3427,113 @@
       <c r="N2" t="s">
         <v>57</v>
       </c>
+      <c r="O2">
+        <v>180</v>
+      </c>
+      <c r="P2">
+        <v>70</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>365</v>
+      </c>
+      <c r="R2" t="s">
+        <v>376</v>
+      </c>
+      <c r="T2" t="s">
+        <v>377</v>
+      </c>
+      <c r="U2" t="s">
+        <v>378</v>
+      </c>
+      <c r="V2" t="s">
+        <v>379</v>
+      </c>
+      <c r="W2" t="s">
+        <v>380</v>
+      </c>
+      <c r="X2" t="s">
+        <v>381</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z2">
+        <v>76567</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>115</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>375</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>68</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="E3" s="2"/>
     </row>
   </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Inavlid Input" error="Please enter 5 digit Zip Code" sqref="E3:E9 E11:E1048576" xr:uid="{190957EF-0EB0-4F09-9E83-4839990B3993}">
+      <formula1>1</formula1>
+      <formula2>5</formula2>
+    </dataValidation>
+    <dataValidation type="whole" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Inavlid Input" error="Please enter 5 digit Zip Code" sqref="E10" xr:uid="{E729A261-EAF0-406F-B3EB-E097B7CE162F}">
+      <formula1>5</formula1>
+    </dataValidation>
+  </dataValidations>
   <hyperlinks>
     <hyperlink ref="L2" r:id="rId1" xr:uid="{52A4A4BE-60D7-4627-A70C-825EB6BDD9E6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Selection" error="Select from the available States" xr:uid="{731E8583-DB9F-45F9-86E0-00F4B4653DF0}">
+          <x14:formula1>
+            <xm:f>'Dropdown Values'!$D$2:$D$55</xm:f>
+          </x14:formula1>
+          <xm:sqref>D2:D1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Selection" error="Please select the Country in the list" xr:uid="{EF18C400-EDCB-4E7A-855B-241554A0857B}">
+          <x14:formula1>
+            <xm:f>'Dropdown Values'!$C$2:$C$254</xm:f>
+          </x14:formula1>
+          <xm:sqref>AB2:AB1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E7BC2500-021D-4F79-9E9B-540F93236936}">
+          <x14:formula1>
+            <xm:f>'Dropdown Values'!$D$2:$D$55</xm:f>
+          </x14:formula1>
+          <xm:sqref>Y2 AC2:AC1048576 AE2:AE1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27982702-2711-473A-A26F-501411054272}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Screenshot funtion has added
</commit_message>
<xml_diff>
--- a/TestData/ApplicationPro_DataFeed.xlsx
+++ b/TestData/ApplicationPro_DataFeed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srinivasa.punnam\PycharmProjects\ApplicationPro\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84E475D3-B89A-4CBF-95B9-CE9C891A2C6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46F5283A-7924-4139-B4AA-BA65FE076F83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{D409B3C3-83F5-4FB1-9D92-4899A37DC1FC}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="383">
   <si>
     <t>UserName</t>
   </si>
@@ -1170,9 +1170,6 @@
     <t>DIRIUT 28376423874</t>
   </si>
   <si>
-    <t>Employed</t>
-  </si>
-  <si>
     <t>ACCOUNTANT</t>
   </si>
   <si>
@@ -1189,6 +1186,9 @@
   </si>
   <si>
     <t>End</t>
+  </si>
+  <si>
+    <t>Retired</t>
   </si>
 </sst>
 </file>
@@ -3249,8 +3249,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{573F1447-AAF6-44E3-84EB-841D47BD4BB3}">
   <dimension ref="A1:AF3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="T3" sqref="T3"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="AE5" sqref="AE5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3437,22 +3437,22 @@
         <v>365</v>
       </c>
       <c r="R2" t="s">
+        <v>382</v>
+      </c>
+      <c r="T2" t="s">
         <v>376</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>377</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>378</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>379</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>380</v>
-      </c>
-      <c r="X2" t="s">
-        <v>381</v>
       </c>
       <c r="Y2" t="s">
         <v>66</v>
@@ -3464,7 +3464,7 @@
         <v>114</v>
       </c>
       <c r="AB2" t="s">
-        <v>115</v>
+        <v>223</v>
       </c>
       <c r="AC2" t="s">
         <v>65</v>
@@ -3472,11 +3472,8 @@
       <c r="AD2" t="s">
         <v>375</v>
       </c>
-      <c r="AE2" t="s">
-        <v>68</v>
-      </c>
       <c r="AF2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
major code is added for ProductSelection.py added exceptions for error handling updated code in other pages
</commit_message>
<xml_diff>
--- a/TestData/ApplicationPro_DataFeed.xlsx
+++ b/TestData/ApplicationPro_DataFeed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srinivasa.punnam\PycharmProjects\ApplicationPro\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46F5283A-7924-4139-B4AA-BA65FE076F83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9237F577-47EA-4711-AD3E-CB6BF76B50A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{D409B3C3-83F5-4FB1-9D92-4899A37DC1FC}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="401">
   <si>
     <t>UserName</t>
   </si>
@@ -147,9 +147,6 @@
     <t>02/17/1991</t>
   </si>
   <si>
-    <t>NextScreen</t>
-  </si>
-  <si>
     <t>CreateNewApplication</t>
   </si>
   <si>
@@ -1189,6 +1186,63 @@
   </si>
   <si>
     <t>Retired</t>
+  </si>
+  <si>
+    <t>Face_Amount</t>
+  </si>
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>Payment_Mode</t>
+  </si>
+  <si>
+    <t>Waiver_of_Premium</t>
+  </si>
+  <si>
+    <t>Accidental_Death_Benefit</t>
+  </si>
+  <si>
+    <t>Accidental_Death_Benefit_Amount</t>
+  </si>
+  <si>
+    <t>Primary_Insured_Rider</t>
+  </si>
+  <si>
+    <t>Primary_Insured_Rider_Amount</t>
+  </si>
+  <si>
+    <t>Childrens_Insurance_Rider</t>
+  </si>
+  <si>
+    <t>Childrens_Insurance_Rider_Units</t>
+  </si>
+  <si>
+    <t>Other_Insured_Rider</t>
+  </si>
+  <si>
+    <t>Next_Screen</t>
+  </si>
+  <si>
+    <t>State_1</t>
+  </si>
+  <si>
+    <t>State_2</t>
+  </si>
+  <si>
+    <t>City_1</t>
+  </si>
+  <si>
+    <t>City_2</t>
+  </si>
+  <si>
+    <t>Choice Non-tobacco</t>
+  </si>
+  <si>
+    <t>Annual</t>
+  </si>
+  <si>
+    <t>ProductSelection</t>
   </si>
 </sst>
 </file>
@@ -1233,10 +1287,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1593,10 +1650,10 @@
         <v>16</v>
       </c>
       <c r="C1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -1607,10 +1664,10 @@
         <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -1621,10 +1678,10 @@
         <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -1635,10 +1692,10 @@
         <v>26</v>
       </c>
       <c r="C4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -1649,10 +1706,10 @@
         <v>27</v>
       </c>
       <c r="C5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -1663,10 +1720,10 @@
         <v>28</v>
       </c>
       <c r="C6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -1677,10 +1734,10 @@
         <v>29</v>
       </c>
       <c r="C7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -1691,10 +1748,10 @@
         <v>30</v>
       </c>
       <c r="C8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -1702,63 +1759,63 @@
         <v>31</v>
       </c>
       <c r="C9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C15" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D16" t="s">
         <v>14</v>
@@ -1766,1309 +1823,1309 @@
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C17" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C19" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D19" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C20" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D20" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D21" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C22" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="23" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C23" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="24" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C24" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D24" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="25" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C25" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="26" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C26" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D26" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="27" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C27" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D27" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="28" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C28" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="29" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C29" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D29" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="30" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C30" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D30" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="31" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C31" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D31" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="32" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C32" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D32" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="33" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C33" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D33" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="34" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C34" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D34" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="35" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C35" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D35" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="36" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C36" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D36" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="37" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C37" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D37" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="38" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C38" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D38" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="39" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C39" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D39" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="40" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C40" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D40" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="41" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C41" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D41" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="42" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C42" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D42" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="43" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C43" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D43" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="44" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C44" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D44" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="45" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C45" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D45" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="46" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C46" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D46" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="47" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C47" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D47" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="48" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C48" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D48" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="49" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C49" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D49" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="50" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C50" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D50" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="51" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C51" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D51" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="52" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C52" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D52" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="53" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C53" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D53" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="54" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C54" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D54" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="55" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C55" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D55" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="56" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C56" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="57" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C57" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="58" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C58" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="59" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C59" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="60" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C60" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="61" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C61" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="62" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C62" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="63" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C63" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="64" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C64" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="65" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C65" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="66" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C66" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="67" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C67" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="68" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C68" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="69" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C69" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="70" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C70" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="71" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C71" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="72" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C72" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="73" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C73" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="74" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C74" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="75" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C75" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="76" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C76" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="77" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C77" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="78" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C78" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="79" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C79" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="80" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C80" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="81" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C81" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="82" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C82" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="83" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C83" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="84" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C84" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="85" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C85" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="86" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C86" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="87" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C87" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="88" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C88" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="89" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C89" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="90" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C90" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="91" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C91" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="92" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C92" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="93" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C93" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="94" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C94" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="95" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C95" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="96" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C96" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="97" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C97" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="98" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C98" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="99" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C99" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="100" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C100" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="101" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C101" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="102" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C102" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="103" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C103" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="104" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C104" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="105" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C105" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="106" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C106" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="107" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C107" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="108" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C108" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="109" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C109" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="110" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C110" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="111" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C111" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="112" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C112" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="113" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C113" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="114" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C114" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="115" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C115" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="116" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C116" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="117" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C117" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="118" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C118" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="119" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C119" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="120" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C120" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="121" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C121" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="122" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C122" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="123" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C123" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="124" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C124" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="125" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C125" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="126" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C126" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="127" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C127" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="128" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C128" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="129" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C129" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="130" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C130" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="131" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C131" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="132" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C132" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="133" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C133" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="134" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C134" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="135" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C135" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="136" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C136" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="137" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C137" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="138" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C138" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="139" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C139" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="140" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C140" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="141" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C141" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="142" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C142" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="143" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C143" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="144" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C144" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="145" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C145" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="146" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C146" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="147" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C147" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="148" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C148" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="149" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C149" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="150" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C150" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="151" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C151" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="152" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C152" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="153" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C153" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="154" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C154" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="155" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C155" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="156" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C156" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="157" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C157" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="158" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C158" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="159" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C159" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="160" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C160" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="161" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C161" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="162" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C162" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="163" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C163" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="164" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C164" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="165" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C165" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="166" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C166" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="167" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C167" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="168" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C168" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="169" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C169" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="170" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C170" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="171" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C171" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="172" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C172" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="173" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C173" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="174" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C174" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="175" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C175" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="176" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C176" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="177" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C177" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="178" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C178" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="179" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C179" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="180" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C180" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="181" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C181" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="182" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C182" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="183" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C183" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="184" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C184" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="185" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C185" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="186" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C186" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="187" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C187" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="188" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C188" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="189" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C189" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="190" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C190" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="191" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C191" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="192" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C192" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="193" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C193" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="194" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C194" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="195" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C195" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="196" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C196" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="197" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C197" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="198" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C198" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="199" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C199" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="200" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C200" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="201" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C201" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="202" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C202" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="203" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C203" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="204" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C204" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="205" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C205" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="206" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C206" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="207" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C207" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="208" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C208" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="209" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C209" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="210" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C210" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="211" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C211" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="212" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C212" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="213" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C213" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="214" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C214" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="215" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C215" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="216" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C216" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="217" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C217" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="218" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C218" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="219" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C219" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="220" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C220" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="221" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C221" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="222" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C222" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="223" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C223" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="224" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C224" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="225" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C225" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="226" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C226" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="227" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C227" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="228" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C228" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="229" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C229" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="230" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C230" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="231" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C231" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="232" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C232" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="233" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C233" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="234" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C234" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="235" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C235" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="236" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C236" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="237" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C237" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="238" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C238" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="239" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C239" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="240" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C240" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="241" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C241" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="242" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C242" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="243" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C243" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="244" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C244" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="245" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C245" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="246" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C246" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="247" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C247" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="248" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C248" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="249" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C249" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="250" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C250" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="251" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C251" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="252" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C252" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="253" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C253" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="254" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C254" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
   </sheetData>
@@ -3081,7 +3138,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3102,7 +3159,7 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>35</v>
+        <v>393</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -3116,7 +3173,7 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -3174,7 +3231,7 @@
         <v>16</v>
       </c>
       <c r="I1" t="s">
-        <v>35</v>
+        <v>393</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -3203,7 +3260,7 @@
         <v>25</v>
       </c>
       <c r="I2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -3249,15 +3306,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{573F1447-AAF6-44E3-84EB-841D47BD4BB3}">
   <dimension ref="A1:AF3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="AE5" sqref="AE5"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.77734375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.33203125" bestFit="1" customWidth="1"/>
@@ -3288,114 +3345,114 @@
   <sheetData>
     <row r="1" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" t="s">
         <v>38</v>
       </c>
-      <c r="B1" t="s">
-        <v>39</v>
-      </c>
       <c r="C1" t="s">
-        <v>40</v>
+        <v>396</v>
       </c>
       <c r="D1" t="s">
+        <v>394</v>
+      </c>
+      <c r="E1" t="s">
         <v>41</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>42</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>43</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>44</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>45</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>46</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>47</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>48</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>49</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>50</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>51</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>52</v>
       </c>
-      <c r="P1" t="s">
-        <v>53</v>
-      </c>
       <c r="Q1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="R1" t="s">
+        <v>365</v>
+      </c>
+      <c r="S1" t="s">
+        <v>57</v>
+      </c>
+      <c r="T1" t="s">
         <v>366</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
+        <v>367</v>
+      </c>
+      <c r="V1" t="s">
+        <v>368</v>
+      </c>
+      <c r="W1" t="s">
+        <v>369</v>
+      </c>
+      <c r="X1" t="s">
+        <v>397</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>395</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA1" t="s">
         <v>58</v>
       </c>
-      <c r="T1" t="s">
-        <v>367</v>
-      </c>
-      <c r="U1" t="s">
-        <v>368</v>
-      </c>
-      <c r="V1" t="s">
-        <v>369</v>
-      </c>
-      <c r="W1" t="s">
+      <c r="AB1" t="s">
         <v>370</v>
       </c>
-      <c r="X1" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>41</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>59</v>
-      </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>371</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>372</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>373</v>
       </c>
-      <c r="AE1" t="s">
-        <v>374</v>
-      </c>
       <c r="AF1" t="s">
-        <v>35</v>
+        <v>393</v>
       </c>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" t="s">
         <v>38</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>39</v>
       </c>
-      <c r="C2" t="s">
-        <v>40</v>
-      </c>
       <c r="D2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E2">
         <v>34534</v>
@@ -3404,10 +3461,10 @@
         <v>6756756765</v>
       </c>
       <c r="G2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I2">
         <v>6756756765</v>
@@ -3416,16 +3473,16 @@
         <v>6756756765</v>
       </c>
       <c r="K2" t="s">
+        <v>54</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="M2">
         <v>789789789</v>
       </c>
       <c r="N2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="O2">
         <v>180</v>
@@ -3434,46 +3491,46 @@
         <v>70</v>
       </c>
       <c r="Q2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="R2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="T2" t="s">
+        <v>375</v>
+      </c>
+      <c r="U2" t="s">
         <v>376</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>377</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>378</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>379</v>
       </c>
-      <c r="X2" t="s">
-        <v>380</v>
-      </c>
       <c r="Y2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="Z2">
         <v>76567</v>
       </c>
       <c r="AA2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AB2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="AC2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AD2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="AF2" t="s">
-        <v>381</v>
+        <v>400</v>
       </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.3">
@@ -3523,14 +3580,107 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27982702-2711-473A-A26F-501411054272}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="12" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.21875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.21875" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.77734375" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.88671875" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>384</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>385</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>386</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>389</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>392</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>200000</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="F2" s="3">
+        <v>5000</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="H2" s="3">
+        <v>5000</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="J2" s="3">
+        <v>5000</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>380</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
modified the existing code added screenshots code for all the screens Updated Execute() function in some screens
</commit_message>
<xml_diff>
--- a/TestData/ApplicationPro_DataFeed.xlsx
+++ b/TestData/ApplicationPro_DataFeed.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srinivasa.punnam\PycharmProjects\ApplicationPro\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BE82086-D673-465A-BFA7-68B38A225F6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ABD1F50-0017-43C9-9A40-47EAF8299635}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15150" yWindow="-16395" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dropdown Values" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="427">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="425">
   <si>
     <t/>
   </si>
@@ -1052,268 +1052,262 @@
     <t>Create New Client</t>
   </si>
   <si>
-    <t>AutoFName</t>
-  </si>
-  <si>
-    <t>AutoLNam</t>
-  </si>
-  <si>
     <t>02/17/1991</t>
   </si>
   <si>
+    <t>PrimaryInsured</t>
+  </si>
+  <si>
+    <t>Primary_Address_Line_1</t>
+  </si>
+  <si>
+    <t>Primary_Address_Line_2</t>
+  </si>
+  <si>
+    <t>City_1</t>
+  </si>
+  <si>
+    <t>State_1</t>
+  </si>
+  <si>
+    <t>Zip_Code</t>
+  </si>
+  <si>
+    <t>Home_Phone</t>
+  </si>
+  <si>
+    <t>Insured_is_Owner</t>
+  </si>
+  <si>
+    <t>Insured_is_Payor</t>
+  </si>
+  <si>
+    <t>Work_Phone</t>
+  </si>
+  <si>
+    <t>Cell_Phone</t>
+  </si>
+  <si>
+    <t>Preferred_Method_of_Contact</t>
+  </si>
+  <si>
+    <t>Email_Address</t>
+  </si>
+  <si>
+    <t>Social_Security_Number</t>
+  </si>
+  <si>
+    <t>Marital_Status</t>
+  </si>
+  <si>
+    <t>Height</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>Tobacco</t>
+  </si>
+  <si>
+    <t>Work_Status</t>
+  </si>
+  <si>
+    <t>Occupational_Duties</t>
+  </si>
+  <si>
+    <t>Employer_Name</t>
+  </si>
+  <si>
+    <t>Employer_Address_Line_1</t>
+  </si>
+  <si>
+    <t>Employer_Address_Line_2</t>
+  </si>
+  <si>
+    <t>City_2</t>
+  </si>
+  <si>
+    <t>State_2</t>
+  </si>
+  <si>
+    <t>Citizenship</t>
+  </si>
+  <si>
+    <t>Country_of_Birth</t>
+  </si>
+  <si>
+    <t>State_of_Birth</t>
+  </si>
+  <si>
+    <t>Driver_License_Number</t>
+  </si>
+  <si>
+    <t>State_of_Issue</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Home Phone</t>
+  </si>
+  <si>
+    <t>test@gmail.com</t>
+  </si>
+  <si>
+    <t>Married</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Retired</t>
+  </si>
+  <si>
+    <t>ACCOUNTANT</t>
+  </si>
+  <si>
+    <t>Deutsche Bank</t>
+  </si>
+  <si>
+    <t>Deutsche Line 1</t>
+  </si>
+  <si>
+    <t>Deutsche Line 2</t>
+  </si>
+  <si>
+    <t>Deutsche City</t>
+  </si>
+  <si>
+    <t>U.S. Citizen</t>
+  </si>
+  <si>
+    <t>DIRIUT 28376423874</t>
+  </si>
+  <si>
+    <t>ProductSelection</t>
+  </si>
+  <si>
+    <t>Face_Amount</t>
+  </si>
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>Payment_Mode</t>
+  </si>
+  <si>
+    <t>Waiver_of_Premium</t>
+  </si>
+  <si>
+    <t>Accidental_Death_Benefit</t>
+  </si>
+  <si>
+    <t>Accidental_Death_Benefit_Amount</t>
+  </si>
+  <si>
+    <t>Primary_Insured_Rider</t>
+  </si>
+  <si>
+    <t>Primary_Insured_Rider_Amount</t>
+  </si>
+  <si>
+    <t>Childrens_Insurance_Rider</t>
+  </si>
+  <si>
+    <t>Childrens_Insurance_Rider_Units</t>
+  </si>
+  <si>
+    <t>Other_Insured_Rider</t>
+  </si>
+  <si>
+    <t>Choice Non-tobacco</t>
+  </si>
+  <si>
+    <t>Annual</t>
+  </si>
+  <si>
+    <t>5000.0</t>
+  </si>
+  <si>
+    <t>Owner</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Relationship</t>
+  </si>
+  <si>
+    <t>Insured</t>
+  </si>
+  <si>
+    <t>Payor</t>
+  </si>
+  <si>
+    <t>Payor Type</t>
+  </si>
+  <si>
+    <t>Beneficiary</t>
+  </si>
+  <si>
+    <t>Beneficiary Level</t>
+  </si>
+  <si>
+    <t>Percentage</t>
+  </si>
+  <si>
+    <t>Estate of Insured</t>
+  </si>
+  <si>
+    <t>Primary</t>
+  </si>
+  <si>
+    <t>ExistingInsurance</t>
+  </si>
+  <si>
+    <t>Existing Insurance</t>
+  </si>
+  <si>
+    <t>PaymentInformation</t>
+  </si>
+  <si>
+    <t>PhysicianInformation</t>
+  </si>
+  <si>
+    <t>Physician Information</t>
+  </si>
+  <si>
+    <t>UnderwritingQuestions</t>
+  </si>
+  <si>
+    <t>Underwriting Questions</t>
+  </si>
+  <si>
+    <t>SupplementalForms</t>
+  </si>
+  <si>
+    <t>Supplemental Forms</t>
+  </si>
+  <si>
+    <t>CompleteApplication</t>
+  </si>
+  <si>
+    <t>Complete Application</t>
+  </si>
+  <si>
+    <t>End</t>
+  </si>
+  <si>
+    <t>Cash With Application</t>
+  </si>
+  <si>
     <t>Male</t>
   </si>
   <si>
-    <t>PrimaryInsured</t>
-  </si>
-  <si>
-    <t>Primary_Address_Line_1</t>
-  </si>
-  <si>
-    <t>Primary_Address_Line_2</t>
-  </si>
-  <si>
-    <t>City_1</t>
-  </si>
-  <si>
-    <t>State_1</t>
-  </si>
-  <si>
-    <t>Zip_Code</t>
-  </si>
-  <si>
-    <t>Home_Phone</t>
-  </si>
-  <si>
-    <t>Insured_is_Owner</t>
-  </si>
-  <si>
-    <t>Insured_is_Payor</t>
-  </si>
-  <si>
-    <t>Work_Phone</t>
-  </si>
-  <si>
-    <t>Cell_Phone</t>
-  </si>
-  <si>
-    <t>Preferred_Method_of_Contact</t>
-  </si>
-  <si>
-    <t>Email_Address</t>
-  </si>
-  <si>
-    <t>Social_Security_Number</t>
-  </si>
-  <si>
-    <t>Marital_Status</t>
-  </si>
-  <si>
-    <t>Height</t>
-  </si>
-  <si>
-    <t>Weight</t>
-  </si>
-  <si>
-    <t>Tobacco</t>
-  </si>
-  <si>
-    <t>Work_Status</t>
-  </si>
-  <si>
-    <t>Occupational_Duties</t>
-  </si>
-  <si>
-    <t>Employer_Name</t>
-  </si>
-  <si>
-    <t>Employer_Address_Line_1</t>
-  </si>
-  <si>
-    <t>Employer_Address_Line_2</t>
-  </si>
-  <si>
-    <t>City_2</t>
-  </si>
-  <si>
-    <t>State_2</t>
-  </si>
-  <si>
-    <t>Citizenship</t>
-  </si>
-  <si>
-    <t>Country_of_Birth</t>
-  </si>
-  <si>
-    <t>State_of_Birth</t>
-  </si>
-  <si>
-    <t>Driver_License_Number</t>
-  </si>
-  <si>
-    <t>State_of_Issue</t>
-  </si>
-  <si>
-    <t>City</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>Home Phone</t>
-  </si>
-  <si>
-    <t>test@gmail.com</t>
-  </si>
-  <si>
-    <t>Married</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Retired</t>
-  </si>
-  <si>
-    <t>ACCOUNTANT</t>
-  </si>
-  <si>
-    <t>Deutsche Bank</t>
-  </si>
-  <si>
-    <t>Deutsche Line 1</t>
-  </si>
-  <si>
-    <t>Deutsche Line 2</t>
-  </si>
-  <si>
-    <t>Deutsche City</t>
-  </si>
-  <si>
-    <t>U.S. Citizen</t>
-  </si>
-  <si>
-    <t>DIRIUT 28376423874</t>
-  </si>
-  <si>
-    <t>ProductSelection</t>
-  </si>
-  <si>
-    <t>Face_Amount</t>
-  </si>
-  <si>
-    <t>Class</t>
-  </si>
-  <si>
-    <t>Payment_Mode</t>
-  </si>
-  <si>
-    <t>Waiver_of_Premium</t>
-  </si>
-  <si>
-    <t>Accidental_Death_Benefit</t>
-  </si>
-  <si>
-    <t>Accidental_Death_Benefit_Amount</t>
-  </si>
-  <si>
-    <t>Primary_Insured_Rider</t>
-  </si>
-  <si>
-    <t>Primary_Insured_Rider_Amount</t>
-  </si>
-  <si>
-    <t>Childrens_Insurance_Rider</t>
-  </si>
-  <si>
-    <t>Childrens_Insurance_Rider_Units</t>
-  </si>
-  <si>
-    <t>Other_Insured_Rider</t>
-  </si>
-  <si>
-    <t>200000.0</t>
-  </si>
-  <si>
-    <t>Choice Non-tobacco</t>
-  </si>
-  <si>
-    <t>Annual</t>
-  </si>
-  <si>
-    <t>5000.0</t>
-  </si>
-  <si>
-    <t>Owner</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Relationship</t>
-  </si>
-  <si>
-    <t>Insured</t>
-  </si>
-  <si>
-    <t>Payor</t>
-  </si>
-  <si>
-    <t>Payor Type</t>
-  </si>
-  <si>
-    <t>Beneficiary</t>
-  </si>
-  <si>
-    <t>Beneficiary Level</t>
-  </si>
-  <si>
-    <t>Percentage</t>
-  </si>
-  <si>
-    <t>Estate of Insured</t>
-  </si>
-  <si>
-    <t>Primary</t>
-  </si>
-  <si>
-    <t>ExistingInsurance</t>
-  </si>
-  <si>
-    <t>Existing Insurance</t>
-  </si>
-  <si>
-    <t>PaymentInformation</t>
-  </si>
-  <si>
-    <t>PhysicianInformation</t>
-  </si>
-  <si>
-    <t>Physician Information</t>
-  </si>
-  <si>
-    <t>UnderwritingQuestions</t>
-  </si>
-  <si>
-    <t>Underwriting Questions</t>
-  </si>
-  <si>
-    <t>SupplementalForms</t>
-  </si>
-  <si>
-    <t>Supplemental Forms</t>
-  </si>
-  <si>
-    <t>CompleteApplication</t>
-  </si>
-  <si>
-    <t>Complete Application</t>
-  </si>
-  <si>
-    <t>End</t>
-  </si>
-  <si>
-    <t>Cash With Application</t>
+    <t>randomname</t>
   </si>
 </sst>
 </file>
@@ -3198,7 +3192,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="B1" t="s">
         <v>327</v>
@@ -3206,10 +3200,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="B2" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
     </row>
   </sheetData>
@@ -3221,9 +3215,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="U6" sqref="U6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -3233,7 +3225,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="B1" t="s">
         <v>327</v>
@@ -3241,10 +3233,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="B2" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
     </row>
   </sheetData>
@@ -3262,7 +3254,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="B1" t="s">
         <v>327</v>
@@ -3270,10 +3262,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="B2" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
     </row>
   </sheetData>
@@ -3291,7 +3283,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="B1" t="s">
         <v>327</v>
@@ -3299,10 +3291,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="B2" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
     </row>
   </sheetData>
@@ -3320,7 +3312,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="B1" t="s">
         <v>327</v>
@@ -3328,10 +3320,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="B2" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
     </row>
   </sheetData>
@@ -3384,9 +3376,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -3422,16 +3427,16 @@
         <v>338</v>
       </c>
       <c r="B2" t="s">
+        <v>424</v>
+      </c>
+      <c r="C2" t="s">
+        <v>424</v>
+      </c>
+      <c r="D2" t="s">
         <v>339</v>
       </c>
-      <c r="C2" t="s">
-        <v>340</v>
-      </c>
-      <c r="D2" t="s">
-        <v>341</v>
-      </c>
       <c r="E2" t="s">
-        <v>342</v>
+        <v>423</v>
       </c>
       <c r="F2" t="s">
         <v>49</v>
@@ -3443,7 +3448,7 @@
         <v>10</v>
       </c>
       <c r="I2" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
     </row>
   </sheetData>
@@ -3455,137 +3460,136 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AF3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="AA22" sqref="AA22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.88671875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.77734375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="23.21875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="15" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="22" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="14.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>341</v>
+      </c>
+      <c r="B1" t="s">
+        <v>342</v>
+      </c>
+      <c r="C1" t="s">
+        <v>343</v>
+      </c>
+      <c r="D1" t="s">
         <v>344</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>345</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>346</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>347</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>348</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>349</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>350</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>351</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>352</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>353</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>354</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>355</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>356</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q1" t="s">
         <v>357</v>
       </c>
-      <c r="O1" t="s">
+      <c r="R1" t="s">
         <v>358</v>
-      </c>
-      <c r="P1" t="s">
-        <v>359</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>360</v>
-      </c>
-      <c r="R1" t="s">
-        <v>361</v>
       </c>
       <c r="S1" t="s">
         <v>249</v>
       </c>
       <c r="T1" t="s">
+        <v>359</v>
+      </c>
+      <c r="U1" t="s">
+        <v>360</v>
+      </c>
+      <c r="V1" t="s">
+        <v>361</v>
+      </c>
+      <c r="W1" t="s">
         <v>362</v>
       </c>
-      <c r="U1" t="s">
+      <c r="X1" t="s">
         <v>363</v>
       </c>
-      <c r="V1" t="s">
+      <c r="Y1" t="s">
         <v>364</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Z1" t="s">
+        <v>345</v>
+      </c>
+      <c r="AA1" t="s">
         <v>365</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AB1" t="s">
         <v>366</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AC1" t="s">
         <v>367</v>
       </c>
-      <c r="Z1" t="s">
-        <v>348</v>
-      </c>
-      <c r="AA1" t="s">
+      <c r="AD1" t="s">
         <v>368</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AE1" t="s">
         <v>369</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>370</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>371</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>372</v>
       </c>
       <c r="AF1" t="s">
         <v>327</v>
@@ -3593,13 +3597,13 @@
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="B2" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="C2" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="D2" t="s">
         <v>111</v>
@@ -3611,10 +3615,10 @@
         <v>9876543210</v>
       </c>
       <c r="G2" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="H2" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="I2">
         <v>9876543210</v>
@@ -3623,16 +3627,16 @@
         <v>9875676881</v>
       </c>
       <c r="K2" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="L2" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="M2">
         <v>789789654</v>
       </c>
       <c r="N2" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="O2">
         <v>180</v>
@@ -3641,25 +3645,25 @@
         <v>70</v>
       </c>
       <c r="Q2" t="s">
+        <v>375</v>
+      </c>
+      <c r="R2" t="s">
+        <v>376</v>
+      </c>
+      <c r="S2" t="s">
+        <v>377</v>
+      </c>
+      <c r="T2" t="s">
         <v>378</v>
       </c>
-      <c r="R2" t="s">
+      <c r="U2" t="s">
         <v>379</v>
       </c>
-      <c r="S2" t="s">
+      <c r="V2" t="s">
         <v>380</v>
       </c>
-      <c r="T2" t="s">
+      <c r="W2" t="s">
         <v>381</v>
-      </c>
-      <c r="U2" t="s">
-        <v>382</v>
-      </c>
-      <c r="V2" t="s">
-        <v>383</v>
-      </c>
-      <c r="W2" t="s">
-        <v>384</v>
       </c>
       <c r="X2" t="s">
         <v>28</v>
@@ -3671,7 +3675,7 @@
         <v>70007</v>
       </c>
       <c r="AA2" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="AB2" t="s">
         <v>182</v>
@@ -3680,13 +3684,13 @@
         <v>24</v>
       </c>
       <c r="AD2" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="AE2" t="s">
         <v>24</v>
       </c>
       <c r="AF2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.3">
@@ -3703,84 +3707,86 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>385</v>
+      </c>
+      <c r="B1" t="s">
+        <v>386</v>
+      </c>
+      <c r="C1" t="s">
+        <v>387</v>
+      </c>
+      <c r="D1" t="s">
         <v>388</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>389</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>390</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>391</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>392</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>393</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>394</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>395</v>
-      </c>
-      <c r="I1" t="s">
-        <v>396</v>
-      </c>
-      <c r="J1" t="s">
-        <v>397</v>
-      </c>
-      <c r="K1" t="s">
-        <v>398</v>
       </c>
       <c r="L1" t="s">
         <v>327</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2">
+        <v>200000</v>
+      </c>
+      <c r="B2" t="s">
+        <v>396</v>
+      </c>
+      <c r="C2" t="s">
+        <v>397</v>
+      </c>
+      <c r="D2" t="s">
+        <v>375</v>
+      </c>
+      <c r="E2" t="s">
+        <v>375</v>
+      </c>
+      <c r="F2" t="s">
+        <v>398</v>
+      </c>
+      <c r="G2" t="s">
+        <v>375</v>
+      </c>
+      <c r="H2" t="s">
+        <v>398</v>
+      </c>
+      <c r="I2" t="s">
+        <v>375</v>
+      </c>
+      <c r="J2" t="s">
+        <v>398</v>
+      </c>
+      <c r="K2" t="s">
+        <v>375</v>
+      </c>
+      <c r="L2" t="s">
         <v>399</v>
-      </c>
-      <c r="B2" t="s">
-        <v>400</v>
-      </c>
-      <c r="C2" t="s">
-        <v>401</v>
-      </c>
-      <c r="D2" t="s">
-        <v>378</v>
-      </c>
-      <c r="E2" t="s">
-        <v>378</v>
-      </c>
-      <c r="F2" t="s">
-        <v>402</v>
-      </c>
-      <c r="G2" t="s">
-        <v>378</v>
-      </c>
-      <c r="H2" t="s">
-        <v>402</v>
-      </c>
-      <c r="I2" t="s">
-        <v>378</v>
-      </c>
-      <c r="J2" t="s">
-        <v>402</v>
-      </c>
-      <c r="K2" t="s">
-        <v>378</v>
-      </c>
-      <c r="L2" t="s">
-        <v>403</v>
       </c>
     </row>
   </sheetData>
@@ -3798,10 +3804,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="B1" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="C1" t="s">
         <v>327</v>
@@ -3809,13 +3815,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>399</v>
+      </c>
+      <c r="B2" t="s">
+        <v>402</v>
+      </c>
+      <c r="C2" t="s">
         <v>403</v>
-      </c>
-      <c r="B2" t="s">
-        <v>406</v>
-      </c>
-      <c r="C2" t="s">
-        <v>407</v>
       </c>
     </row>
   </sheetData>
@@ -3833,7 +3839,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="B1" t="s">
         <v>327</v>
@@ -3841,10 +3847,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="B2" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
     </row>
   </sheetData>
@@ -3857,26 +3863,23 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="B1" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="C1" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="D1" t="s">
         <v>327</v>
@@ -3884,16 +3887,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="B2" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="C2">
         <v>100</v>
       </c>
       <c r="D2" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
     </row>
   </sheetData>
@@ -3911,7 +3914,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="B1" t="s">
         <v>327</v>
@@ -3919,10 +3922,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="B2" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the code and removed wait time in between the screens
</commit_message>
<xml_diff>
--- a/TestData/ApplicationPro_DataFeed.xlsx
+++ b/TestData/ApplicationPro_DataFeed.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srinivasa.punnam\PycharmProjects\ApplicationPro\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ABD1F50-0017-43C9-9A40-47EAF8299635}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43BB9A19-D093-4A0F-A910-E8777201F3E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="10" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dropdown Values" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="425">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="426">
   <si>
     <t/>
   </si>
@@ -1052,6 +1052,12 @@
     <t>Create New Client</t>
   </si>
   <si>
+    <t>AutoFName</t>
+  </si>
+  <si>
+    <t>AutoLNam</t>
+  </si>
+  <si>
     <t>02/17/1991</t>
   </si>
   <si>
@@ -1305,9 +1311,6 @@
   </si>
   <si>
     <t>Male</t>
-  </si>
-  <si>
-    <t>randomname</t>
   </si>
 </sst>
 </file>
@@ -3192,7 +3195,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="B1" t="s">
         <v>327</v>
@@ -3200,10 +3203,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="B2" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
     </row>
   </sheetData>
@@ -3225,7 +3228,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="B1" t="s">
         <v>327</v>
@@ -3233,10 +3236,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="B2" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
     </row>
   </sheetData>
@@ -3254,7 +3257,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="B1" t="s">
         <v>327</v>
@@ -3262,10 +3265,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="B2" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
     </row>
   </sheetData>
@@ -3283,7 +3286,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="B1" t="s">
         <v>327</v>
@@ -3291,10 +3294,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="B2" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
     </row>
   </sheetData>
@@ -3306,13 +3309,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="B1" t="s">
         <v>327</v>
@@ -3320,10 +3323,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="B2" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
     </row>
   </sheetData>
@@ -3376,22 +3379,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -3427,16 +3419,16 @@
         <v>338</v>
       </c>
       <c r="B2" t="s">
-        <v>424</v>
+        <v>339</v>
       </c>
       <c r="C2" t="s">
-        <v>424</v>
+        <v>340</v>
       </c>
       <c r="D2" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="E2" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="F2" t="s">
         <v>49</v>
@@ -3448,7 +3440,7 @@
         <v>10</v>
       </c>
       <c r="I2" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
     </row>
   </sheetData>
@@ -3499,97 +3491,97 @@
   <sheetData>
     <row r="1" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="B1" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="C1" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="D1" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="E1" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="F1" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="G1" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="H1" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="I1" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="J1" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="K1" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="L1" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="M1" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="N1" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="O1" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="P1" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="Q1" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="R1" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="S1" t="s">
         <v>249</v>
       </c>
       <c r="T1" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="U1" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="V1" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="W1" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="X1" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="Y1" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="Z1" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="AA1" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="AB1" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="AC1" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="AD1" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="AE1" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="AF1" t="s">
         <v>327</v>
@@ -3597,13 +3589,13 @@
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="B2" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="C2" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="D2" t="s">
         <v>111</v>
@@ -3615,10 +3607,10 @@
         <v>9876543210</v>
       </c>
       <c r="G2" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="H2" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="I2">
         <v>9876543210</v>
@@ -3627,16 +3619,16 @@
         <v>9875676881</v>
       </c>
       <c r="K2" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="L2" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="M2">
         <v>789789654</v>
       </c>
       <c r="N2" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="O2">
         <v>180</v>
@@ -3645,25 +3637,25 @@
         <v>70</v>
       </c>
       <c r="Q2" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="R2" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="S2" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="T2" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="U2" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="V2" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="W2" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="X2" t="s">
         <v>28</v>
@@ -3675,7 +3667,7 @@
         <v>70007</v>
       </c>
       <c r="AA2" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="AB2" t="s">
         <v>182</v>
@@ -3684,13 +3676,13 @@
         <v>24</v>
       </c>
       <c r="AD2" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="AE2" t="s">
         <v>24</v>
       </c>
       <c r="AF2" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.3">
@@ -3715,37 +3707,37 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="B1" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="C1" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="D1" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="E1" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="F1" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="G1" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="H1" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="I1" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="J1" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="K1" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="L1" t="s">
         <v>327</v>
@@ -3756,37 +3748,37 @@
         <v>200000</v>
       </c>
       <c r="B2" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="C2" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="D2" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="E2" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="F2" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="G2" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="H2" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="I2" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="J2" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="K2" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="L2" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
     </row>
   </sheetData>
@@ -3804,10 +3796,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="B1" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="C1" t="s">
         <v>327</v>
@@ -3815,13 +3807,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="B2" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="C2" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
     </row>
   </sheetData>
@@ -3839,7 +3831,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="B1" t="s">
         <v>327</v>
@@ -3847,10 +3839,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="B2" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
     </row>
   </sheetData>
@@ -3873,13 +3865,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="B1" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="C1" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="D1" t="s">
         <v>327</v>
@@ -3887,16 +3879,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="B2" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="C2">
         <v>100</v>
       </c>
       <c r="D2" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
     </row>
   </sheetData>
@@ -3914,7 +3906,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="B1" t="s">
         <v>327</v>
@@ -3922,10 +3914,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="B2" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
     </row>
   </sheetData>

</xml_diff>